<commit_message>
fix:  quitar el cons dentro de la columnas de fechas
</commit_message>
<xml_diff>
--- a/ai_model/data/Template Plannink (1).xlsx
+++ b/ai_model/data/Template Plannink (1).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chamba\Repositorio\Prueba-frontend-kpital\ai_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chamba\Repositorio\Kpital-sistema-inventario\ai_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDC49C9-41D0-4721-A991-EE6B040599EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F99CD-AD0D-4D57-A92F-16322DEF10C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9CF0F399-52F7-43AC-B800-CC92B24E8CD0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9CF0F399-52F7-43AC-B800-CC92B24E8CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="16ABR V2590" sheetId="1" r:id="rId1"/>
@@ -336,90 +336,6 @@
     <t>STOCK  TOTAL</t>
   </si>
   <si>
-    <t>CONS ENE
-2023</t>
-  </si>
-  <si>
-    <t>CONS FEB
-2023</t>
-  </si>
-  <si>
-    <t>CONS MAR
-2023</t>
-  </si>
-  <si>
-    <t>CONS ABR
-2023</t>
-  </si>
-  <si>
-    <t>CONS MAY
-2023</t>
-  </si>
-  <si>
-    <t>CONS JUN
-2023</t>
-  </si>
-  <si>
-    <t>CONS JUL
-2023</t>
-  </si>
-  <si>
-    <t>CONS AGO
-2023</t>
-  </si>
-  <si>
-    <t>CONS SEP
-2023</t>
-  </si>
-  <si>
-    <t>CONS OCT
-2023</t>
-  </si>
-  <si>
-    <t>CONS NOV
-2023</t>
-  </si>
-  <si>
-    <t>CONS DIC
-2023</t>
-  </si>
-  <si>
-    <t>CONS ENE
-2024</t>
-  </si>
-  <si>
-    <t>CONS FEB
-2024</t>
-  </si>
-  <si>
-    <t>CONS MAR
-2024</t>
-  </si>
-  <si>
-    <t>CONS ABR
-2024</t>
-  </si>
-  <si>
-    <t>CONS MAY
-2024</t>
-  </si>
-  <si>
-    <t>CONS JUN
-2024</t>
-  </si>
-  <si>
-    <t>CONS JUL
-2024</t>
-  </si>
-  <si>
-    <t>CONS AGO
-2024</t>
-  </si>
-  <si>
-    <t>CONS SEP
-2024</t>
-  </si>
-  <si>
     <t>PROM CONS+Proyec</t>
   </si>
   <si>
@@ -919,38 +835,122 @@
     <t>V531-D</t>
   </si>
   <si>
-    <t>CONS OCT
+    <t>UNIDADES EN TRANSITO</t>
+  </si>
+  <si>
+    <t>STOCK  INICIAL</t>
+  </si>
+  <si>
+    <t>ENE
+2023</t>
+  </si>
+  <si>
+    <t>FEB
+2023</t>
+  </si>
+  <si>
+    <t>MAR
+2023</t>
+  </si>
+  <si>
+    <t>ABR
+2023</t>
+  </si>
+  <si>
+    <t>MAY
+2023</t>
+  </si>
+  <si>
+    <t>JUN
+2023</t>
+  </si>
+  <si>
+    <t>JUL
+2023</t>
+  </si>
+  <si>
+    <t>AGO
+2023</t>
+  </si>
+  <si>
+    <t>SEP
+2023</t>
+  </si>
+  <si>
+    <t>OCT
+2023</t>
+  </si>
+  <si>
+    <t>NOV
+2023</t>
+  </si>
+  <si>
+    <t>DIC
+2023</t>
+  </si>
+  <si>
+    <t>ENE
 2024</t>
   </si>
   <si>
-    <t>CONS NOV
+    <t>FEB
 2024</t>
   </si>
   <si>
-    <t>CONS DIC
+    <t>MAR
 2024</t>
   </si>
   <si>
-    <t>CONS ENE
+    <t>ABR
+2024</t>
+  </si>
+  <si>
+    <t>MAY
+2024</t>
+  </si>
+  <si>
+    <t>JUN
+2024</t>
+  </si>
+  <si>
+    <t>JUL
+2024</t>
+  </si>
+  <si>
+    <t>AGO
+2024</t>
+  </si>
+  <si>
+    <t>SEP
+2024</t>
+  </si>
+  <si>
+    <t>NOV
+2024</t>
+  </si>
+  <si>
+    <t>OCT
+2024</t>
+  </si>
+  <si>
+    <t>DIC
+2024</t>
+  </si>
+  <si>
+    <t>ENE
 2025</t>
   </si>
   <si>
-    <t>CONS FEB
+    <t>FEB
 2025</t>
   </si>
   <si>
-    <t>CONS MAR
+    <t>MAR
 2025</t>
   </si>
   <si>
-    <t>CONS ABR
+    <t>ABR
 2025</t>
-  </si>
-  <si>
-    <t>UNIDADES EN TRANSITO</t>
-  </si>
-  <si>
-    <t>STOCK  INICIAL</t>
   </si>
 </sst>
 </file>
@@ -1788,27 +1788,27 @@
   </sheetPr>
   <dimension ref="A1:AM202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="4.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" style="4" customWidth="1"/>
-    <col min="5" max="25" width="6.33203125" style="14" customWidth="1"/>
-    <col min="26" max="32" width="4.77734375" style="14" customWidth="1"/>
-    <col min="33" max="34" width="9.44140625" style="14" customWidth="1"/>
-    <col min="35" max="35" width="6.6640625" style="14" customWidth="1"/>
-    <col min="36" max="36" width="6.6640625" style="14" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="7.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="4" customWidth="1"/>
+    <col min="5" max="25" width="6.28515625" style="14" customWidth="1"/>
+    <col min="26" max="32" width="4.7109375" style="14" customWidth="1"/>
+    <col min="33" max="34" width="9.42578125" style="14" customWidth="1"/>
+    <col min="35" max="35" width="6.7109375" style="14" customWidth="1"/>
+    <col min="36" max="36" width="6.7109375" style="14" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="7.7109375" style="1" customWidth="1"/>
     <col min="38" max="38" width="8" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="11.44140625" style="1"/>
+    <col min="39" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="57"/>
       <c r="C1" s="3"/>
@@ -1846,7 +1846,7 @@
       <c r="AJ1" s="6"/>
       <c r="AL1" s="7"/>
     </row>
-    <row r="2" spans="1:39" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>45762</v>
       </c>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="AL2" s="16"/>
     </row>
-    <row r="3" spans="1:39" s="17" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" s="17" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
@@ -1899,120 +1899,120 @@
         <v>3</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA3" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="AB3" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC3" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD3" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF3" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="AG3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="21" t="s">
+      <c r="AH3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="AJ3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="AK3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N3" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="W3" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y3" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z3" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="AA3" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB3" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="AC3" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="AD3" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="AE3" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF3" s="21" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="AH3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI3" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK3" s="24" t="s">
-        <v>30</v>
-      </c>
       <c r="AL3" s="25" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="AM3" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C4" s="29">
         <v>6</v>
@@ -2131,12 +2131,12 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C5" s="29">
         <v>6</v>
@@ -2255,12 +2255,12 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C6" s="29">
         <v>6</v>
@@ -2379,12 +2379,12 @@
         <v>910</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C7" s="29">
         <v>6</v>
@@ -2503,12 +2503,12 @@
         <v>507</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C8" s="29">
         <v>12</v>
@@ -2627,12 +2627,12 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C9" s="29">
         <v>9</v>
@@ -2749,12 +2749,12 @@
         <v>327</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C10" s="29">
         <v>6</v>
@@ -2873,12 +2873,12 @@
         <v>482</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C11" s="29">
         <v>6</v>
@@ -2997,12 +2997,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C12" s="29">
         <v>6</v>
@@ -3121,12 +3121,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C13" s="29">
         <v>6</v>
@@ -3245,12 +3245,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C14" s="29">
         <v>6</v>
@@ -3369,12 +3369,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C15" s="29">
         <v>6</v>
@@ -3493,12 +3493,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C16" s="29">
         <v>6</v>
@@ -3617,12 +3617,12 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C17" s="29">
         <v>6</v>
@@ -3741,12 +3741,12 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C18" s="29">
         <v>6</v>
@@ -3865,12 +3865,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C19" s="29">
         <v>6</v>
@@ -3989,12 +3989,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C20" s="29">
         <v>6</v>
@@ -4113,12 +4113,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C21" s="29">
         <v>6</v>
@@ -4237,12 +4237,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C22" s="29">
         <v>6</v>
@@ -4361,12 +4361,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C23" s="29">
         <v>6</v>
@@ -4485,12 +4485,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C24" s="29">
         <v>6</v>
@@ -4609,12 +4609,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C25" s="29">
         <v>12</v>
@@ -4731,12 +4731,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C26" s="29">
         <v>6</v>
@@ -4855,12 +4855,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C27" s="29">
         <v>2</v>
@@ -4979,12 +4979,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C28" s="29">
         <v>6</v>
@@ -5101,12 +5101,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C29" s="29">
         <v>6</v>
@@ -5223,12 +5223,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C30" s="29">
         <v>12</v>
@@ -5345,12 +5345,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C31" s="29">
         <v>6</v>
@@ -5469,12 +5469,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="48" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C32" s="29">
         <v>6</v>
@@ -5591,12 +5591,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C33" s="29">
         <v>6</v>
@@ -5715,12 +5715,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C34" s="29">
         <v>6</v>
@@ -5839,12 +5839,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C35" s="29">
         <v>6</v>
@@ -5963,12 +5963,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C36" s="29">
         <v>9</v>
@@ -6087,12 +6087,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C37" s="29">
         <v>6</v>
@@ -6211,12 +6211,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C38" s="29">
         <v>6</v>
@@ -6335,12 +6335,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C39" s="29">
         <v>6</v>
@@ -6457,12 +6457,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B40" s="40" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C40" s="29">
         <v>6</v>
@@ -6579,12 +6579,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C41" s="29">
         <v>6</v>
@@ -6701,12 +6701,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C42" s="29">
         <v>6</v>
@@ -6823,12 +6823,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C43" s="29">
         <v>6</v>
@@ -6947,12 +6947,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C44" s="29">
         <v>6</v>
@@ -7071,12 +7071,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C45" s="29">
         <v>6</v>
@@ -7195,12 +7195,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C46" s="29">
         <v>6</v>
@@ -7317,12 +7317,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C47" s="29">
         <v>6</v>
@@ -7441,12 +7441,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B48" s="28" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C48" s="29">
         <v>6</v>
@@ -7565,12 +7565,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="26" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C49" s="29">
         <v>6</v>
@@ -7687,12 +7687,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B50" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C50" s="29">
         <v>6</v>
@@ -7811,12 +7811,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C51" s="29">
         <v>6</v>
@@ -7933,12 +7933,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="B52" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C52" s="29">
         <v>6</v>
@@ -8057,12 +8057,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B53" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C53" s="29">
         <v>6</v>
@@ -8179,12 +8179,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C54" s="29">
         <v>6</v>
@@ -8301,12 +8301,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="26" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C55" s="29">
         <v>6</v>
@@ -8423,12 +8423,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C56" s="29">
         <v>6</v>
@@ -8547,12 +8547,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C57" s="29">
         <v>6</v>
@@ -8671,12 +8671,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C58" s="29">
         <v>6</v>
@@ -8793,12 +8793,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="46" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C59" s="29">
         <v>6</v>
@@ -8915,12 +8915,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="46" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B60" s="28" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C60" s="29">
         <v>12</v>
@@ -9037,12 +9037,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="46" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C61" s="29">
         <v>6</v>
@@ -9161,12 +9161,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="50" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C62" s="29">
         <v>6</v>
@@ -9283,12 +9283,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="50" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C63" s="29">
         <v>6</v>
@@ -9405,12 +9405,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="50" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C64" s="29">
         <v>6</v>
@@ -9527,12 +9527,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="50" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B65" s="40" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C65" s="29">
         <v>6</v>
@@ -9649,12 +9649,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="46" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C66" s="29">
         <v>12</v>
@@ -9771,12 +9771,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="50" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C67" s="29">
         <v>6</v>
@@ -9893,12 +9893,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="50" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C68" s="29">
         <v>1</v>
@@ -10017,12 +10017,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="50" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C69" s="29">
         <v>6</v>
@@ -10139,12 +10139,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="51" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C70" s="29">
         <v>6</v>
@@ -10261,12 +10261,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="50" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B71" s="40" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C71" s="29">
         <v>6</v>
@@ -10385,12 +10385,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="52" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B72" s="28" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C72" s="29">
         <v>12</v>
@@ -10507,12 +10507,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="50" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C73" s="29">
         <v>6</v>
@@ -10629,12 +10629,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="50" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C74" s="29">
         <v>6</v>
@@ -10751,12 +10751,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="50" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B75" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C75" s="29">
         <v>6</v>
@@ -10873,12 +10873,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="46" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C76" s="29">
         <v>6</v>
@@ -10995,12 +10995,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="46" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C77" s="29">
         <v>6</v>
@@ -11117,12 +11117,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="50" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C78" s="29">
         <v>6</v>
@@ -11239,12 +11239,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="50" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C79" s="29">
         <v>6</v>
@@ -11363,12 +11363,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="26" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B80" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C80" s="29">
         <v>6</v>
@@ -11485,12 +11485,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="46" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="B81" s="28" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C81" s="29">
         <v>6</v>
@@ -11607,12 +11607,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="50" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="B82" s="39" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C82" s="29">
         <v>6</v>
@@ -11729,12 +11729,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="46" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B83" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C83" s="29">
         <v>6</v>
@@ -11851,12 +11851,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="46" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B84" s="28" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C84" s="29">
         <v>12</v>
@@ -11973,12 +11973,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="46" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C85" s="29">
         <v>6</v>
@@ -12095,12 +12095,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B86" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C86" s="29">
         <v>6</v>
@@ -12217,12 +12217,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B87" s="28" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C87" s="29">
         <v>12</v>
@@ -12339,12 +12339,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B88" s="28" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C88" s="29">
         <v>6</v>
@@ -12461,12 +12461,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="46" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C89" s="29">
         <v>9</v>
@@ -12583,12 +12583,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="46" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B90" s="28" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C90" s="29">
         <v>6</v>
@@ -12705,12 +12705,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="46" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C91" s="43">
         <v>6</v>
@@ -12827,12 +12827,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="53" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C92" s="29">
         <v>6</v>
@@ -12949,12 +12949,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="46" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B93" s="39" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C93" s="29">
         <v>12</v>
@@ -13071,12 +13071,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="27" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B94" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C94" s="29">
         <v>6</v>
@@ -13193,12 +13193,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B95" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C95" s="29">
         <v>6</v>
@@ -13315,12 +13315,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="27" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C96" s="29">
         <v>6</v>
@@ -13437,12 +13437,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C97" s="29">
         <v>6</v>
@@ -13559,12 +13559,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C98" s="29">
         <v>9</v>
@@ -13681,12 +13681,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B99" s="28" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C99" s="29">
         <v>6</v>
@@ -13803,12 +13803,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="46" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="B100" s="28" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C100" s="29">
         <v>6</v>
@@ -13925,12 +13925,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="B101" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C101" s="29">
         <v>6</v>
@@ -14047,12 +14047,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B102" s="28" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C102" s="29">
         <v>6</v>
@@ -14169,12 +14169,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="B103" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C103" s="29">
         <v>6</v>
@@ -14291,12 +14291,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="55" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B104" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C104" s="29">
         <v>6</v>
@@ -14413,12 +14413,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="54" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C105" s="29">
         <v>6</v>
@@ -14535,12 +14535,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C106" s="29">
         <v>12</v>
@@ -14657,12 +14657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="46" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B107" s="28" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C107" s="29">
         <v>6</v>
@@ -14779,12 +14779,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="46" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B108" s="40" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="C108" s="29">
         <v>6</v>
@@ -14901,12 +14901,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="46" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C109" s="29">
         <v>6</v>
@@ -15023,12 +15023,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="46" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C110" s="29">
         <v>9</v>
@@ -15145,12 +15145,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="46" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="B111" s="39" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C111" s="29">
         <v>6</v>
@@ -15267,12 +15267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="46" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C112" s="29">
         <v>6</v>
@@ -15389,12 +15389,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="46" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C113" s="29">
         <v>6</v>
@@ -15511,12 +15511,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="46" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C114" s="29">
         <v>6</v>
@@ -15633,12 +15633,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="46" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C115" s="29">
         <v>6</v>
@@ -15755,12 +15755,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="46" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="B116" s="28" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C116" s="29">
         <v>6</v>
@@ -15877,9 +15877,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="46" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="B117" s="28"/>
       <c r="C117" s="29">
@@ -15983,12 +15983,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="46" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C118" s="29">
         <v>9</v>
@@ -16105,12 +16105,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="46" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="B119" s="39" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C119" s="29">
         <v>6</v>
@@ -16227,12 +16227,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="46" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C120" s="29">
         <v>9</v>
@@ -16349,12 +16349,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="46" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C121" s="29">
         <v>1</v>
@@ -16471,12 +16471,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:39" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="50" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C122" s="29">
         <v>6</v>
@@ -16593,12 +16593,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="46" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B123" s="28" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C123" s="29">
         <v>6</v>
@@ -16715,12 +16715,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:39" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="46" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B124" s="28" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C124" s="29">
         <v>6</v>
@@ -16837,7 +16837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="125" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="4"/>
@@ -16877,7 +16877,7 @@
       <c r="AK125" s="1"/>
       <c r="AL125" s="1"/>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -16911,7 +16911,7 @@
       <c r="AI126" s="1"/>
       <c r="AJ126" s="1"/>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
@@ -16945,7 +16945,7 @@
       <c r="AI127" s="1"/>
       <c r="AJ127" s="1"/>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:39" x14ac:dyDescent="0.25">
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -16979,7 +16979,7 @@
       <c r="AI128" s="1"/>
       <c r="AJ128" s="1"/>
     </row>
-    <row r="129" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="129" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -17013,7 +17013,7 @@
       <c r="AI129" s="1"/>
       <c r="AJ129" s="1"/>
     </row>
-    <row r="130" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="130" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -17047,7 +17047,7 @@
       <c r="AI130" s="1"/>
       <c r="AJ130" s="1"/>
     </row>
-    <row r="131" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="131" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -17081,7 +17081,7 @@
       <c r="AI131" s="1"/>
       <c r="AJ131" s="1"/>
     </row>
-    <row r="132" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="132" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -17115,7 +17115,7 @@
       <c r="AI132" s="1"/>
       <c r="AJ132" s="1"/>
     </row>
-    <row r="133" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="133" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -17149,7 +17149,7 @@
       <c r="AI133" s="1"/>
       <c r="AJ133" s="1"/>
     </row>
-    <row r="134" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="134" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
@@ -17183,7 +17183,7 @@
       <c r="AI134" s="1"/>
       <c r="AJ134" s="1"/>
     </row>
-    <row r="135" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="135" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -17217,7 +17217,7 @@
       <c r="AI135" s="1"/>
       <c r="AJ135" s="1"/>
     </row>
-    <row r="136" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="136" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
@@ -17251,7 +17251,7 @@
       <c r="AI136" s="1"/>
       <c r="AJ136" s="1"/>
     </row>
-    <row r="137" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="137" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
@@ -17285,7 +17285,7 @@
       <c r="AI137" s="1"/>
       <c r="AJ137" s="1"/>
     </row>
-    <row r="138" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
@@ -17319,7 +17319,7 @@
       <c r="AI138" s="1"/>
       <c r="AJ138" s="1"/>
     </row>
-    <row r="139" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="139" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
@@ -17353,7 +17353,7 @@
       <c r="AI139" s="1"/>
       <c r="AJ139" s="1"/>
     </row>
-    <row r="140" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="140" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
@@ -17387,7 +17387,7 @@
       <c r="AI140" s="1"/>
       <c r="AJ140" s="1"/>
     </row>
-    <row r="141" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="141" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
@@ -17421,7 +17421,7 @@
       <c r="AI141" s="1"/>
       <c r="AJ141" s="1"/>
     </row>
-    <row r="142" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="142" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
@@ -17455,7 +17455,7 @@
       <c r="AI142" s="1"/>
       <c r="AJ142" s="1"/>
     </row>
-    <row r="143" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="143" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
@@ -17489,7 +17489,7 @@
       <c r="AI143" s="1"/>
       <c r="AJ143" s="1"/>
     </row>
-    <row r="144" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="144" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
@@ -17523,7 +17523,7 @@
       <c r="AI144" s="1"/>
       <c r="AJ144" s="1"/>
     </row>
-    <row r="145" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="145" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
@@ -17557,7 +17557,7 @@
       <c r="AI145" s="1"/>
       <c r="AJ145" s="1"/>
     </row>
-    <row r="146" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="146" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
@@ -17591,7 +17591,7 @@
       <c r="AI146" s="1"/>
       <c r="AJ146" s="1"/>
     </row>
-    <row r="147" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="147" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -17625,7 +17625,7 @@
       <c r="AI147" s="1"/>
       <c r="AJ147" s="1"/>
     </row>
-    <row r="148" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="148" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
@@ -17659,7 +17659,7 @@
       <c r="AI148" s="1"/>
       <c r="AJ148" s="1"/>
     </row>
-    <row r="149" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="149" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
@@ -17693,7 +17693,7 @@
       <c r="AI149" s="1"/>
       <c r="AJ149" s="1"/>
     </row>
-    <row r="150" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="150" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
@@ -17727,7 +17727,7 @@
       <c r="AI150" s="1"/>
       <c r="AJ150" s="1"/>
     </row>
-    <row r="151" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="151" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -17761,7 +17761,7 @@
       <c r="AI151" s="1"/>
       <c r="AJ151" s="1"/>
     </row>
-    <row r="152" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="152" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
@@ -17795,7 +17795,7 @@
       <c r="AI152" s="1"/>
       <c r="AJ152" s="1"/>
     </row>
-    <row r="153" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="153" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
@@ -17829,7 +17829,7 @@
       <c r="AI153" s="1"/>
       <c r="AJ153" s="1"/>
     </row>
-    <row r="154" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="154" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
@@ -17863,7 +17863,7 @@
       <c r="AI154" s="1"/>
       <c r="AJ154" s="1"/>
     </row>
-    <row r="155" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="155" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
@@ -17897,7 +17897,7 @@
       <c r="AI155" s="1"/>
       <c r="AJ155" s="1"/>
     </row>
-    <row r="156" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="156" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
@@ -17931,7 +17931,7 @@
       <c r="AI156" s="1"/>
       <c r="AJ156" s="1"/>
     </row>
-    <row r="157" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="157" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
@@ -17965,7 +17965,7 @@
       <c r="AI157" s="1"/>
       <c r="AJ157" s="1"/>
     </row>
-    <row r="158" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="158" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
@@ -17999,7 +17999,7 @@
       <c r="AI158" s="1"/>
       <c r="AJ158" s="1"/>
     </row>
-    <row r="159" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="159" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
@@ -18033,7 +18033,7 @@
       <c r="AI159" s="1"/>
       <c r="AJ159" s="1"/>
     </row>
-    <row r="160" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="160" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
@@ -18067,7 +18067,7 @@
       <c r="AI160" s="1"/>
       <c r="AJ160" s="1"/>
     </row>
-    <row r="161" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="161" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
@@ -18101,7 +18101,7 @@
       <c r="AI161" s="1"/>
       <c r="AJ161" s="1"/>
     </row>
-    <row r="162" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="162" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
@@ -18135,7 +18135,7 @@
       <c r="AI162" s="1"/>
       <c r="AJ162" s="1"/>
     </row>
-    <row r="163" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="163" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
@@ -18169,7 +18169,7 @@
       <c r="AI163" s="1"/>
       <c r="AJ163" s="1"/>
     </row>
-    <row r="164" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="164" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
@@ -18203,7 +18203,7 @@
       <c r="AI164" s="1"/>
       <c r="AJ164" s="1"/>
     </row>
-    <row r="165" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="165" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
@@ -18237,7 +18237,7 @@
       <c r="AI165" s="1"/>
       <c r="AJ165" s="1"/>
     </row>
-    <row r="166" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="166" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
@@ -18271,7 +18271,7 @@
       <c r="AI166" s="1"/>
       <c r="AJ166" s="1"/>
     </row>
-    <row r="167" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="167" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
@@ -18305,7 +18305,7 @@
       <c r="AI167" s="1"/>
       <c r="AJ167" s="1"/>
     </row>
-    <row r="168" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="168" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
@@ -18339,7 +18339,7 @@
       <c r="AI168" s="1"/>
       <c r="AJ168" s="1"/>
     </row>
-    <row r="169" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="169" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
@@ -18373,7 +18373,7 @@
       <c r="AI169" s="1"/>
       <c r="AJ169" s="1"/>
     </row>
-    <row r="170" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="170" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
@@ -18407,7 +18407,7 @@
       <c r="AI170" s="1"/>
       <c r="AJ170" s="1"/>
     </row>
-    <row r="171" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="171" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E171" s="1"/>
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
@@ -18441,7 +18441,7 @@
       <c r="AI171" s="1"/>
       <c r="AJ171" s="1"/>
     </row>
-    <row r="172" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="172" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
@@ -18475,7 +18475,7 @@
       <c r="AI172" s="1"/>
       <c r="AJ172" s="1"/>
     </row>
-    <row r="173" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="173" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E173" s="1"/>
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
@@ -18509,7 +18509,7 @@
       <c r="AI173" s="1"/>
       <c r="AJ173" s="1"/>
     </row>
-    <row r="174" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="174" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
@@ -18543,7 +18543,7 @@
       <c r="AI174" s="1"/>
       <c r="AJ174" s="1"/>
     </row>
-    <row r="175" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="175" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
@@ -18577,7 +18577,7 @@
       <c r="AI175" s="1"/>
       <c r="AJ175" s="1"/>
     </row>
-    <row r="176" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="176" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E176" s="1"/>
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
@@ -18611,7 +18611,7 @@
       <c r="AI176" s="1"/>
       <c r="AJ176" s="1"/>
     </row>
-    <row r="177" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="177" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E177" s="1"/>
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
@@ -18645,7 +18645,7 @@
       <c r="AI177" s="1"/>
       <c r="AJ177" s="1"/>
     </row>
-    <row r="178" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="178" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
@@ -18679,7 +18679,7 @@
       <c r="AI178" s="1"/>
       <c r="AJ178" s="1"/>
     </row>
-    <row r="179" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="179" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E179" s="1"/>
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
@@ -18713,7 +18713,7 @@
       <c r="AI179" s="1"/>
       <c r="AJ179" s="1"/>
     </row>
-    <row r="180" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="180" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E180" s="1"/>
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
@@ -18747,7 +18747,7 @@
       <c r="AI180" s="1"/>
       <c r="AJ180" s="1"/>
     </row>
-    <row r="181" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="181" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E181" s="1"/>
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
@@ -18781,7 +18781,7 @@
       <c r="AI181" s="1"/>
       <c r="AJ181" s="1"/>
     </row>
-    <row r="182" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="182" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E182" s="1"/>
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
@@ -18815,7 +18815,7 @@
       <c r="AI182" s="1"/>
       <c r="AJ182" s="1"/>
     </row>
-    <row r="183" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="183" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E183" s="1"/>
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
@@ -18849,7 +18849,7 @@
       <c r="AI183" s="1"/>
       <c r="AJ183" s="1"/>
     </row>
-    <row r="184" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="184" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E184" s="1"/>
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
@@ -18883,7 +18883,7 @@
       <c r="AI184" s="1"/>
       <c r="AJ184" s="1"/>
     </row>
-    <row r="185" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="185" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E185" s="1"/>
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
@@ -18917,7 +18917,7 @@
       <c r="AI185" s="1"/>
       <c r="AJ185" s="1"/>
     </row>
-    <row r="186" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="186" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E186" s="1"/>
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
@@ -18951,7 +18951,7 @@
       <c r="AI186" s="1"/>
       <c r="AJ186" s="1"/>
     </row>
-    <row r="187" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="187" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E187" s="1"/>
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
@@ -18985,7 +18985,7 @@
       <c r="AI187" s="1"/>
       <c r="AJ187" s="1"/>
     </row>
-    <row r="188" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="188" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E188" s="1"/>
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
@@ -19019,7 +19019,7 @@
       <c r="AI188" s="1"/>
       <c r="AJ188" s="1"/>
     </row>
-    <row r="189" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="189" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E189" s="1"/>
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
@@ -19053,7 +19053,7 @@
       <c r="AI189" s="1"/>
       <c r="AJ189" s="1"/>
     </row>
-    <row r="190" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="190" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
@@ -19087,7 +19087,7 @@
       <c r="AI190" s="1"/>
       <c r="AJ190" s="1"/>
     </row>
-    <row r="191" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="191" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
@@ -19121,7 +19121,7 @@
       <c r="AI191" s="1"/>
       <c r="AJ191" s="1"/>
     </row>
-    <row r="192" spans="5:36" x14ac:dyDescent="0.3">
+    <row r="192" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E192" s="1"/>
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
@@ -19155,7 +19155,7 @@
       <c r="AI192" s="1"/>
       <c r="AJ192" s="1"/>
     </row>
-    <row r="193" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E193" s="1"/>
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
@@ -19189,7 +19189,7 @@
       <c r="AI193" s="1"/>
       <c r="AJ193" s="1"/>
     </row>
-    <row r="194" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E194" s="1"/>
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
@@ -19223,7 +19223,7 @@
       <c r="AI194" s="1"/>
       <c r="AJ194" s="1"/>
     </row>
-    <row r="195" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E195" s="1"/>
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
@@ -19257,7 +19257,7 @@
       <c r="AI195" s="1"/>
       <c r="AJ195" s="1"/>
     </row>
-    <row r="196" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E196" s="1"/>
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
@@ -19291,7 +19291,7 @@
       <c r="AI196" s="1"/>
       <c r="AJ196" s="1"/>
     </row>
-    <row r="197" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E197" s="1"/>
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
@@ -19325,7 +19325,7 @@
       <c r="AI197" s="1"/>
       <c r="AJ197" s="1"/>
     </row>
-    <row r="198" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E198" s="1"/>
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
@@ -19359,7 +19359,7 @@
       <c r="AI198" s="1"/>
       <c r="AJ198" s="1"/>
     </row>
-    <row r="199" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:38" x14ac:dyDescent="0.25">
       <c r="E199" s="1"/>
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
@@ -19393,7 +19393,7 @@
       <c r="AI199" s="1"/>
       <c r="AJ199" s="1"/>
     </row>
-    <row r="200" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1"/>
       <c r="B200" s="1"/>
       <c r="C200" s="4"/>
@@ -19401,7 +19401,7 @@
       <c r="AK200" s="1"/>
       <c r="AL200" s="1"/>
     </row>
-    <row r="201" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
       <c r="B201" s="1"/>
       <c r="C201" s="4"/>
@@ -19409,7 +19409,7 @@
       <c r="AK201" s="1"/>
       <c r="AL201" s="1"/>
     </row>
-    <row r="202" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:38" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1"/>
       <c r="B202" s="1"/>
       <c r="C202" s="4"/>

</xml_diff>